<commit_message>
Update nginx and port pre-processing
</commit_message>
<xml_diff>
--- a/module/flo/homeassistant/src/build/resources/entity_metadata.xlsx
+++ b/module/flo/homeassistant/src/build/resources/entity_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graham/Code/asystem/module/flo/homeassistant/src/build/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687AD324-A7FD-FD4D-9225-7CA7036DE5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7538CF6E-3508-864A-800C-70CFB63A17A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="2760" windowWidth="40680" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5014" uniqueCount="1146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4994" uniqueCount="1140">
   <si>
     <t>index</t>
   </si>
@@ -3450,12 +3450,6 @@
     <t>connection_alias_target</t>
   </si>
   <si>
-    <t>Alias</t>
-  </si>
-  <si>
-    <t>zigbee2mqtt</t>
-  </si>
-  <si>
     <t>connection_alias</t>
   </si>
   <si>
@@ -3463,18 +3457,6 @@
   </si>
   <si>
     <t>Target for the host name  connection_alias</t>
-  </si>
-  <si>
-    <t>vernemq</t>
-  </si>
-  <si>
-    <t>influxdb</t>
-  </si>
-  <si>
-    <t>plex</t>
-  </si>
-  <si>
-    <t>weewx</t>
   </si>
 </sst>
 </file>
@@ -3677,7 +3659,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3814,39 +3796,31 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="48">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri (Body)"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3881,25 +3855,6 @@
         <name val="Calibri (Body)"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri (Body)"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4786,10 +4741,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A3:AS700" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46">
-  <autoFilter ref="A3:AS700" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AS700">
-    <sortCondition ref="A3:A700"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A3:AS695" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46">
+  <autoFilter ref="A3:AS695" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AS695">
+    <sortCondition ref="A3:A695"/>
   </sortState>
   <tableColumns count="45">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="index" dataDxfId="44"/>
@@ -4840,9 +4795,9 @@
     <tableColumn id="36" xr3:uid="{9BE9D8F1-8323-CD41-9A9F-7BB21381C895}" name="connection_vlan" dataDxfId="5"/>
     <tableColumn id="35" xr3:uid="{083AE619-8F32-3D45-8483-3D0D4C3918AF}" name="connection_mac" dataDxfId="4"/>
     <tableColumn id="34" xr3:uid="{BBD927E3-6295-6C4D-8EC3-6DFFCC064F3B}" name="connection_ip" dataDxfId="3"/>
-    <tableColumn id="45" xr3:uid="{D2505BB0-619A-2448-99AC-1B6A79A8476A}" name="connection_alias" dataDxfId="0"/>
+    <tableColumn id="45" xr3:uid="{D2505BB0-619A-2448-99AC-1B6A79A8476A}" name="connection_alias" dataDxfId="2"/>
     <tableColumn id="44" xr3:uid="{973C04E6-70FB-B842-B649-19B754996AB1}" name="connection_alias_target" dataDxfId="1"/>
-    <tableColumn id="33" xr3:uid="{02BC701A-79AC-534B-9960-6F231D2962E3}" name="device_connections" dataDxfId="2">
+    <tableColumn id="33" xr3:uid="{02BC701A-79AC-534B-9960-6F231D2962E3}" name="device_connections" dataDxfId="0">
       <calculatedColumnFormula>IF(AND(ISBLANK(AO4), ISBLANK(AP4)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO4), "", _xlfn.CONCAT("[""mac"", """, AO4, """]")), IF(ISBLANK(AP4), "", _xlfn.CONCAT(", [""ip"", """, AP4, """]")), "]"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5147,10 +5102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS700"/>
+  <dimension ref="A1:AS695"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK336" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="AQ373" sqref="AQ373"/>
+    <sheetView tabSelected="1" topLeftCell="A336" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="A369" sqref="A369:XFD373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5466,10 +5421,10 @@
         <v>463</v>
       </c>
       <c r="AQ2" s="26" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="AR2" s="28" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="AS2" s="28" t="s">
         <v>1129</v>
@@ -5603,7 +5558,7 @@
         <v>462</v>
       </c>
       <c r="AQ3" s="5" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="AR3" s="5" t="s">
         <v>1136</v>
@@ -13925,8 +13880,7 @@
         <v>488</v>
       </c>
       <c r="AP103" s="12"/>
-      <c r="AQ103" s="48"/>
-      <c r="AR103" s="48"/>
+      <c r="AQ103" s="8"/>
       <c r="AS103" s="8" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -29473,8 +29427,7 @@
       </c>
       <c r="AF320" s="39"/>
       <c r="AP320" s="12"/>
-      <c r="AQ320" s="48"/>
-      <c r="AR320" s="48"/>
+      <c r="AQ320" s="8"/>
       <c r="AS320" s="8" t="str">
         <f t="shared" si="29"/>
         <v/>
@@ -29647,8 +29600,8 @@
       <c r="AP322" s="13" t="s">
         <v>659</v>
       </c>
-      <c r="AQ322" s="49"/>
-      <c r="AR322" s="49"/>
+      <c r="AQ322" s="14"/>
+      <c r="AR322" s="14"/>
       <c r="AS322" s="8" t="str">
         <f t="shared" si="29"/>
         <v>[["mac", "90:dd:5d:ce:1e:96"], ["ip", "10.0.4.47"]]</v>
@@ -29790,8 +29743,7 @@
       </c>
       <c r="AF324" s="39"/>
       <c r="AP324" s="12"/>
-      <c r="AQ324" s="48"/>
-      <c r="AR324" s="48"/>
+      <c r="AQ324" s="8"/>
       <c r="AS324" s="8" t="str">
         <f t="shared" si="29"/>
         <v/>
@@ -29878,8 +29830,8 @@
       <c r="AP325" s="13" t="s">
         <v>921</v>
       </c>
-      <c r="AQ325" s="49"/>
-      <c r="AR325" s="49"/>
+      <c r="AQ325" s="14"/>
+      <c r="AR325" s="14"/>
       <c r="AS325" s="8" t="str">
         <f t="shared" si="29"/>
         <v>[["mac", "38:42:0b:47:73:dc"], ["ip", "10.0.4.43"]]</v>
@@ -29966,8 +29918,8 @@
       <c r="AP326" s="13" t="s">
         <v>688</v>
       </c>
-      <c r="AQ326" s="49"/>
-      <c r="AR326" s="49"/>
+      <c r="AQ326" s="14"/>
+      <c r="AR326" s="14"/>
       <c r="AS326" s="8" t="str">
         <f t="shared" si="29"/>
         <v>[["mac", "48:a6:b8:e2:50:40"], ["ip", "10.0.4.41"]]</v>
@@ -30054,8 +30006,8 @@
       <c r="AP327" s="13" t="s">
         <v>689</v>
       </c>
-      <c r="AQ327" s="49"/>
-      <c r="AR327" s="49"/>
+      <c r="AQ327" s="14"/>
+      <c r="AR327" s="14"/>
       <c r="AS327" s="8" t="str">
         <f t="shared" si="29"/>
         <v>[["mac", "5c:aa:fd:f1:a3:d4"], ["ip", "10.0.4.42"]]</v>
@@ -30229,8 +30181,8 @@
       <c r="AP329" s="13" t="s">
         <v>660</v>
       </c>
-      <c r="AQ329" s="49"/>
-      <c r="AR329" s="49"/>
+      <c r="AQ329" s="14"/>
+      <c r="AR329" s="14"/>
       <c r="AS329" s="8" t="str">
         <f t="shared" si="29"/>
         <v>[["mac", "d4:a3:3d:5c:8c:28"], ["ip", "10.0.4.48"]]</v>
@@ -31378,7 +31330,7 @@
       <c r="U347" s="8"/>
       <c r="Z347" s="10"/>
       <c r="AB347" s="8" t="str">
-        <f t="shared" ref="AB347:AB415" si="32">IF(ISBLANK(AA347),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C347), "/", E347, "/config"))</f>
+        <f t="shared" ref="AB347:AB410" si="32">IF(ISBLANK(AA347),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C347), "/", E347, "/config"))</f>
         <v/>
       </c>
       <c r="AC347" s="8" t="str">
@@ -32399,8 +32351,8 @@
       <c r="AP363" s="13" t="s">
         <v>581</v>
       </c>
-      <c r="AQ363" s="49"/>
-      <c r="AR363" s="49"/>
+      <c r="AQ363" s="14"/>
+      <c r="AR363" s="14"/>
       <c r="AS363" s="8" t="str">
         <f t="shared" si="29"/>
         <v>[["mac", "00:e0:4c:68:07:0d"], ["ip", "10.0.2.13"]]</v>
@@ -32465,8 +32417,8 @@
       <c r="AP364" s="13" t="s">
         <v>859</v>
       </c>
-      <c r="AQ364" s="49"/>
-      <c r="AR364" s="49"/>
+      <c r="AQ364" s="14"/>
+      <c r="AR364" s="14"/>
       <c r="AS364" s="8" t="str">
         <f t="shared" si="29"/>
         <v>[["mac", "40:6c:8f:2a:da:9c"], ["ip", "10.0.2.14"]]</v>
@@ -32531,8 +32483,8 @@
       <c r="AP365" s="13" t="s">
         <v>933</v>
       </c>
-      <c r="AQ365" s="49"/>
-      <c r="AR365" s="49"/>
+      <c r="AQ365" s="14"/>
+      <c r="AR365" s="14"/>
       <c r="AS365" s="8" t="str">
         <f t="shared" si="29"/>
         <v>[["mac", "0c:4d:e9:d2:86:6c"], ["ip", "10.0.2.15"]]</v>
@@ -32597,8 +32549,8 @@
       <c r="AP366" s="13" t="s">
         <v>934</v>
       </c>
-      <c r="AQ366" s="49"/>
-      <c r="AR366" s="49"/>
+      <c r="AQ366" s="14"/>
+      <c r="AR366" s="14"/>
       <c r="AS366" s="8" t="str">
         <f t="shared" si="29"/>
         <v>[["mac", "b8:27:eb:78:74:0e"], ["ip", "10.0.2.16"]]</v>
@@ -32735,350 +32687,179 @@
       </c>
     </row>
     <row r="369" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A369" s="50">
-        <v>5200</v>
-      </c>
-      <c r="B369" s="50" t="s">
+      <c r="A369" s="8">
+        <v>6000</v>
+      </c>
+      <c r="B369" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C369" s="50" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D369" s="50"/>
-      <c r="E369" s="51"/>
-      <c r="F369" s="52" t="str">
+      <c r="C369" s="8" t="s">
+        <v>842</v>
+      </c>
+      <c r="F369" s="8" t="str">
         <f>IF(ISBLANK(E369), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
-      <c r="G369" s="50"/>
-      <c r="H369" s="50"/>
-      <c r="I369" s="51"/>
-      <c r="J369" s="50"/>
-      <c r="K369" s="50"/>
-      <c r="M369" s="50"/>
-      <c r="N369" s="50"/>
-      <c r="O369" s="50"/>
-      <c r="P369" s="53"/>
-      <c r="Q369" s="53"/>
-      <c r="R369" s="53"/>
-      <c r="S369" s="53"/>
-      <c r="T369" s="53"/>
-      <c r="U369" s="50"/>
-      <c r="V369" s="50"/>
-      <c r="W369" s="50"/>
-      <c r="X369" s="50"/>
-      <c r="Y369" s="50"/>
-      <c r="Z369" s="53"/>
-      <c r="AA369" s="50"/>
-      <c r="AB369" s="50" t="str">
-        <f>IF(ISBLANK(AA369),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C369), "/", E369, "/config"))</f>
-        <v/>
-      </c>
-      <c r="AC369" s="50" t="str">
-        <f>IF(ISBLANK(AA369),  "", _xlfn.CONCAT(LOWER(C369), "/", E369))</f>
-        <v/>
-      </c>
-      <c r="AD369" s="50"/>
-      <c r="AE369" s="50"/>
-      <c r="AF369" s="54"/>
-      <c r="AG369" s="50"/>
-      <c r="AH369" s="55"/>
-      <c r="AI369" s="56"/>
-      <c r="AJ369" s="56"/>
-      <c r="AK369" s="50"/>
-      <c r="AL369" s="50"/>
-      <c r="AN369" s="50"/>
-      <c r="AO369" s="50"/>
-      <c r="AP369" s="50"/>
-      <c r="AQ369" s="8" t="s">
-        <v>1138</v>
-      </c>
-      <c r="AR369" s="8" t="s">
-        <v>863</v>
-      </c>
-      <c r="AS369" s="52" t="str">
-        <f>IF(AND(ISBLANK(AO369), ISBLANK(AP369)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO369), "", _xlfn.CONCAT("[""mac"", """, AO369, """]")), IF(ISBLANK(AP369), "", _xlfn.CONCAT(", [""ip"", """, AP369, """]")), "]"))</f>
-        <v/>
+      <c r="O369" s="8"/>
+      <c r="P369" s="10"/>
+      <c r="Q369" s="10"/>
+      <c r="R369" s="10"/>
+      <c r="S369" s="10"/>
+      <c r="T369" s="10"/>
+      <c r="U369" s="8"/>
+      <c r="Z369" s="10"/>
+      <c r="AB369" s="8" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AC369" s="8" t="str">
+        <f t="shared" ref="AC369:AC432" si="33">IF(ISBLANK(AA369),  "", _xlfn.CONCAT(LOWER(C369), "/", E369))</f>
+        <v/>
+      </c>
+      <c r="AF369" s="39"/>
+      <c r="AG369" s="8" t="s">
+        <v>681</v>
+      </c>
+      <c r="AN369" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="AO369" s="8" t="s">
+        <v>682</v>
+      </c>
+      <c r="AP369" s="8"/>
+      <c r="AQ369" s="8"/>
+      <c r="AS369" s="8" t="str">
+        <f t="shared" ref="AS369:AS432" si="34">IF(AND(ISBLANK(AO369), ISBLANK(AP369)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO369), "", _xlfn.CONCAT("[""mac"", """, AO369, """]")), IF(ISBLANK(AP369), "", _xlfn.CONCAT(", [""ip"", """, AP369, """]")), "]"))</f>
+        <v>[["mac", "bc:09:63:42:09:c0"]]</v>
       </c>
     </row>
     <row r="370" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A370" s="50">
-        <v>5201</v>
-      </c>
-      <c r="B370" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C370" s="50" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D370" s="50"/>
-      <c r="E370" s="51"/>
-      <c r="F370" s="52" t="str">
+      <c r="F370" s="8" t="str">
         <f>IF(ISBLANK(E370), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
-      <c r="G370" s="50"/>
-      <c r="H370" s="50"/>
-      <c r="I370" s="51"/>
-      <c r="J370" s="50"/>
-      <c r="K370" s="50"/>
-      <c r="M370" s="50"/>
-      <c r="N370" s="50"/>
-      <c r="O370" s="50"/>
-      <c r="P370" s="53"/>
-      <c r="Q370" s="53"/>
-      <c r="R370" s="53"/>
-      <c r="S370" s="53"/>
-      <c r="T370" s="53"/>
-      <c r="U370" s="50"/>
-      <c r="V370" s="50"/>
-      <c r="W370" s="50"/>
-      <c r="X370" s="50"/>
-      <c r="Y370" s="50"/>
-      <c r="Z370" s="53"/>
-      <c r="AA370" s="50"/>
-      <c r="AB370" s="50" t="str">
-        <f>IF(ISBLANK(AA370),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C370), "/", E370, "/config"))</f>
-        <v/>
-      </c>
-      <c r="AC370" s="50" t="str">
-        <f>IF(ISBLANK(AA370),  "", _xlfn.CONCAT(LOWER(C370), "/", E370))</f>
-        <v/>
-      </c>
-      <c r="AD370" s="50"/>
-      <c r="AE370" s="50"/>
-      <c r="AF370" s="54"/>
-      <c r="AG370" s="50"/>
-      <c r="AH370" s="55"/>
-      <c r="AI370" s="56"/>
-      <c r="AJ370" s="56"/>
-      <c r="AK370" s="50"/>
-      <c r="AL370" s="50"/>
-      <c r="AN370" s="50"/>
-      <c r="AO370" s="50"/>
-      <c r="AP370" s="50"/>
-      <c r="AQ370" s="8" t="s">
-        <v>1142</v>
-      </c>
-      <c r="AR370" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="AS370" s="52" t="str">
-        <f>IF(AND(ISBLANK(AO370), ISBLANK(AP370)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO370), "", _xlfn.CONCAT("[""mac"", """, AO370, """]")), IF(ISBLANK(AP370), "", _xlfn.CONCAT(", [""ip"", """, AP370, """]")), "]"))</f>
+      <c r="O370" s="8"/>
+      <c r="P370" s="10"/>
+      <c r="Q370" s="10"/>
+      <c r="R370" s="10"/>
+      <c r="S370" s="10"/>
+      <c r="T370" s="10"/>
+      <c r="U370" s="8"/>
+      <c r="Z370" s="10"/>
+      <c r="AB370" s="8" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AC370" s="8" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AF370" s="39"/>
+      <c r="AP370" s="8"/>
+      <c r="AQ370" s="8"/>
+      <c r="AS370" s="8" t="str">
+        <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
     <row r="371" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A371" s="50">
-        <v>5202</v>
-      </c>
-      <c r="B371" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C371" s="50" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D371" s="50"/>
-      <c r="E371" s="51"/>
-      <c r="F371" s="52" t="str">
+      <c r="B371" s="14"/>
+      <c r="C371" s="14"/>
+      <c r="D371" s="14"/>
+      <c r="E371" s="14"/>
+      <c r="F371" s="8" t="str">
         <f>IF(ISBLANK(E371), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
-      <c r="G371" s="50"/>
-      <c r="H371" s="50"/>
-      <c r="I371" s="51"/>
-      <c r="J371" s="50"/>
-      <c r="K371" s="50"/>
-      <c r="M371" s="50"/>
-      <c r="N371" s="50"/>
-      <c r="O371" s="50"/>
-      <c r="P371" s="53"/>
-      <c r="Q371" s="53"/>
-      <c r="R371" s="53"/>
-      <c r="S371" s="53"/>
-      <c r="T371" s="53"/>
-      <c r="U371" s="50"/>
-      <c r="V371" s="50"/>
-      <c r="W371" s="50"/>
-      <c r="X371" s="50"/>
-      <c r="Y371" s="50"/>
-      <c r="Z371" s="53"/>
-      <c r="AA371" s="50"/>
-      <c r="AB371" s="50" t="str">
-        <f>IF(ISBLANK(AA371),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C371), "/", E371, "/config"))</f>
-        <v/>
-      </c>
-      <c r="AC371" s="50" t="str">
-        <f>IF(ISBLANK(AA371),  "", _xlfn.CONCAT(LOWER(C371), "/", E371))</f>
-        <v/>
-      </c>
-      <c r="AD371" s="50"/>
-      <c r="AE371" s="50"/>
-      <c r="AF371" s="54"/>
-      <c r="AG371" s="50"/>
-      <c r="AH371" s="55"/>
-      <c r="AI371" s="56"/>
-      <c r="AJ371" s="56"/>
-      <c r="AK371" s="50"/>
-      <c r="AL371" s="50"/>
-      <c r="AN371" s="50"/>
-      <c r="AO371" s="50"/>
-      <c r="AP371" s="50"/>
-      <c r="AQ371" s="8" t="s">
-        <v>1143</v>
-      </c>
-      <c r="AR371" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="AS371" s="52" t="str">
-        <f>IF(AND(ISBLANK(AO371), ISBLANK(AP371)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO371), "", _xlfn.CONCAT("[""mac"", """, AO371, """]")), IF(ISBLANK(AP371), "", _xlfn.CONCAT(", [""ip"", """, AP371, """]")), "]"))</f>
+      <c r="G371" s="14"/>
+      <c r="H371" s="14"/>
+      <c r="I371" s="14"/>
+      <c r="K371" s="14"/>
+      <c r="L371" s="14"/>
+      <c r="M371" s="14"/>
+      <c r="O371" s="8"/>
+      <c r="P371" s="10"/>
+      <c r="Q371" s="10"/>
+      <c r="R371" s="10"/>
+      <c r="S371" s="10"/>
+      <c r="T371" s="10"/>
+      <c r="U371" s="8"/>
+      <c r="Z371" s="10"/>
+      <c r="AB371" s="8" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AC371" s="8" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AF371" s="39"/>
+      <c r="AP371" s="8"/>
+      <c r="AQ371" s="8"/>
+      <c r="AS371" s="8" t="str">
+        <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
     <row r="372" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A372" s="50">
-        <v>5203</v>
-      </c>
-      <c r="B372" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C372" s="50" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D372" s="50"/>
-      <c r="E372" s="51"/>
-      <c r="F372" s="52" t="str">
+      <c r="F372" s="8" t="str">
         <f>IF(ISBLANK(E372), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
-      <c r="G372" s="50"/>
-      <c r="H372" s="50"/>
-      <c r="I372" s="51"/>
-      <c r="J372" s="50"/>
-      <c r="K372" s="50"/>
-      <c r="M372" s="50"/>
-      <c r="N372" s="50"/>
-      <c r="O372" s="50"/>
-      <c r="P372" s="53"/>
-      <c r="Q372" s="53"/>
-      <c r="R372" s="53"/>
-      <c r="S372" s="53"/>
-      <c r="T372" s="53"/>
-      <c r="U372" s="50"/>
-      <c r="V372" s="50"/>
-      <c r="W372" s="50"/>
-      <c r="X372" s="50"/>
-      <c r="Y372" s="50"/>
-      <c r="Z372" s="53"/>
-      <c r="AA372" s="50"/>
-      <c r="AB372" s="50" t="str">
-        <f>IF(ISBLANK(AA372),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C372), "/", E372, "/config"))</f>
-        <v/>
-      </c>
-      <c r="AC372" s="50" t="str">
-        <f>IF(ISBLANK(AA372),  "", _xlfn.CONCAT(LOWER(C372), "/", E372))</f>
-        <v/>
-      </c>
-      <c r="AD372" s="50"/>
-      <c r="AE372" s="50"/>
-      <c r="AF372" s="54"/>
-      <c r="AG372" s="50"/>
-      <c r="AH372" s="55"/>
-      <c r="AI372" s="56"/>
-      <c r="AJ372" s="56"/>
-      <c r="AK372" s="50"/>
-      <c r="AL372" s="50"/>
-      <c r="AN372" s="50"/>
-      <c r="AO372" s="50"/>
-      <c r="AP372" s="50"/>
-      <c r="AQ372" s="8" t="s">
-        <v>1144</v>
-      </c>
-      <c r="AR372" s="8" t="s">
-        <v>928</v>
-      </c>
-      <c r="AS372" s="52" t="str">
-        <f>IF(AND(ISBLANK(AO372), ISBLANK(AP372)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO372), "", _xlfn.CONCAT("[""mac"", """, AO372, """]")), IF(ISBLANK(AP372), "", _xlfn.CONCAT(", [""ip"", """, AP372, """]")), "]"))</f>
+      <c r="O372" s="8"/>
+      <c r="P372" s="10"/>
+      <c r="Q372" s="10"/>
+      <c r="R372" s="10"/>
+      <c r="S372" s="10"/>
+      <c r="T372" s="10"/>
+      <c r="U372" s="8"/>
+      <c r="Z372" s="10"/>
+      <c r="AB372" s="8" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AC372" s="8" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AF372" s="39"/>
+      <c r="AP372" s="8"/>
+      <c r="AQ372" s="8"/>
+      <c r="AS372" s="8" t="str">
+        <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
     <row r="373" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A373" s="50">
-        <v>5204</v>
-      </c>
-      <c r="B373" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C373" s="50" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D373" s="50"/>
-      <c r="E373" s="51"/>
-      <c r="F373" s="52" t="str">
+      <c r="F373" s="8" t="str">
         <f>IF(ISBLANK(E373), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
-      <c r="G373" s="50"/>
-      <c r="H373" s="50"/>
-      <c r="I373" s="51"/>
-      <c r="J373" s="50"/>
-      <c r="K373" s="50"/>
-      <c r="M373" s="50"/>
-      <c r="N373" s="50"/>
-      <c r="O373" s="50"/>
-      <c r="P373" s="53"/>
-      <c r="Q373" s="53"/>
-      <c r="R373" s="53"/>
-      <c r="S373" s="53"/>
-      <c r="T373" s="53"/>
-      <c r="U373" s="50"/>
-      <c r="V373" s="50"/>
-      <c r="W373" s="50"/>
-      <c r="X373" s="50"/>
-      <c r="Y373" s="50"/>
-      <c r="Z373" s="53"/>
-      <c r="AA373" s="50"/>
-      <c r="AB373" s="50" t="str">
-        <f>IF(ISBLANK(AA373),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C373), "/", E373, "/config"))</f>
-        <v/>
-      </c>
-      <c r="AC373" s="50" t="str">
-        <f>IF(ISBLANK(AA373),  "", _xlfn.CONCAT(LOWER(C373), "/", E373))</f>
-        <v/>
-      </c>
-      <c r="AD373" s="50"/>
-      <c r="AE373" s="50"/>
-      <c r="AF373" s="54"/>
-      <c r="AG373" s="50"/>
-      <c r="AH373" s="55"/>
-      <c r="AI373" s="56"/>
-      <c r="AJ373" s="56"/>
-      <c r="AK373" s="50"/>
-      <c r="AL373" s="50"/>
-      <c r="AN373" s="50"/>
-      <c r="AO373" s="50"/>
-      <c r="AP373" s="50"/>
-      <c r="AQ373" s="8" t="s">
-        <v>1145</v>
-      </c>
-      <c r="AR373" s="8" t="s">
-        <v>863</v>
-      </c>
-      <c r="AS373" s="52" t="str">
-        <f>IF(AND(ISBLANK(AO373), ISBLANK(AP373)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO373), "", _xlfn.CONCAT("[""mac"", """, AO373, """]")), IF(ISBLANK(AP373), "", _xlfn.CONCAT(", [""ip"", """, AP373, """]")), "]"))</f>
+      <c r="O373" s="8"/>
+      <c r="P373" s="10"/>
+      <c r="Q373" s="10"/>
+      <c r="R373" s="10"/>
+      <c r="S373" s="10"/>
+      <c r="T373" s="10"/>
+      <c r="U373" s="8"/>
+      <c r="Z373" s="10"/>
+      <c r="AB373" s="8" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AC373" s="8" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AF373" s="39"/>
+      <c r="AP373" s="8"/>
+      <c r="AQ373" s="8"/>
+      <c r="AS373" s="8" t="str">
+        <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
     <row r="374" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A374" s="8">
-        <v>6000</v>
-      </c>
-      <c r="B374" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C374" s="8" t="s">
-        <v>842</v>
-      </c>
       <c r="F374" s="8" t="str">
         <f>IF(ISBLANK(E374), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
@@ -33096,24 +32877,15 @@
         <v/>
       </c>
       <c r="AC374" s="8" t="str">
-        <f t="shared" ref="AC374:AC437" si="33">IF(ISBLANK(AA374),  "", _xlfn.CONCAT(LOWER(C374), "/", E374))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="AF374" s="39"/>
-      <c r="AG374" s="8" t="s">
-        <v>681</v>
-      </c>
-      <c r="AN374" s="8" t="s">
-        <v>605</v>
-      </c>
-      <c r="AO374" s="8" t="s">
-        <v>682</v>
-      </c>
       <c r="AP374" s="8"/>
       <c r="AQ374" s="8"/>
       <c r="AS374" s="8" t="str">
-        <f t="shared" ref="AS374:AS437" si="34">IF(AND(ISBLANK(AO374), ISBLANK(AP374)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO374), "", _xlfn.CONCAT("[""mac"", """, AO374, """]")), IF(ISBLANK(AP374), "", _xlfn.CONCAT(", [""ip"", """, AP374, """]")), "]"))</f>
-        <v>[["mac", "bc:09:63:42:09:c0"]]</v>
+        <f t="shared" si="34"/>
+        <v/>
       </c>
     </row>
     <row r="375" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -33146,20 +32918,11 @@
       </c>
     </row>
     <row r="376" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B376" s="14"/>
-      <c r="C376" s="14"/>
-      <c r="D376" s="14"/>
-      <c r="E376" s="14"/>
+      <c r="E376" s="12"/>
       <c r="F376" s="8" t="str">
         <f>IF(ISBLANK(E376), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
-      <c r="G376" s="14"/>
-      <c r="H376" s="14"/>
-      <c r="I376" s="14"/>
-      <c r="K376" s="14"/>
-      <c r="L376" s="14"/>
-      <c r="M376" s="14"/>
       <c r="O376" s="8"/>
       <c r="P376" s="10"/>
       <c r="Q376" s="10"/>
@@ -33185,6 +32948,7 @@
       </c>
     </row>
     <row r="377" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E377" s="12"/>
       <c r="F377" s="8" t="str">
         <f>IF(ISBLANK(E377), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
@@ -33301,7 +33065,6 @@
       </c>
     </row>
     <row r="381" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E381" s="12"/>
       <c r="F381" s="8" t="str">
         <f>IF(ISBLANK(E381), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
@@ -33331,7 +33094,6 @@
       </c>
     </row>
     <row r="382" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E382" s="12"/>
       <c r="F382" s="8" t="str">
         <f>IF(ISBLANK(E382), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
@@ -34135,7 +33897,7 @@
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AF409" s="39"/>
+      <c r="AF409" s="38"/>
       <c r="AP409" s="8"/>
       <c r="AQ409" s="8"/>
       <c r="AS409" s="8" t="str">
@@ -34186,14 +33948,14 @@
       <c r="U411" s="8"/>
       <c r="Z411" s="10"/>
       <c r="AB411" s="8" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="AB411:AB474" si="35">IF(ISBLANK(AA411),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C411), "/", E411, "/config"))</f>
         <v/>
       </c>
       <c r="AC411" s="8" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AF411" s="39"/>
+      <c r="AF411" s="38"/>
       <c r="AP411" s="8"/>
       <c r="AQ411" s="8"/>
       <c r="AS411" s="8" t="str">
@@ -34215,14 +33977,14 @@
       <c r="U412" s="8"/>
       <c r="Z412" s="10"/>
       <c r="AB412" s="8" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="AC412" s="8" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AF412" s="39"/>
+      <c r="AF412" s="38"/>
       <c r="AP412" s="8"/>
       <c r="AQ412" s="8"/>
       <c r="AS412" s="8" t="str">
@@ -34244,14 +34006,14 @@
       <c r="U413" s="8"/>
       <c r="Z413" s="10"/>
       <c r="AB413" s="8" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="AC413" s="8" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AF413" s="39"/>
+      <c r="AF413" s="38"/>
       <c r="AP413" s="8"/>
       <c r="AQ413" s="8"/>
       <c r="AS413" s="8" t="str">
@@ -34273,14 +34035,14 @@
       <c r="U414" s="8"/>
       <c r="Z414" s="10"/>
       <c r="AB414" s="8" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="AC414" s="8" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AF414" s="38"/>
+      <c r="AF414" s="39"/>
       <c r="AP414" s="8"/>
       <c r="AQ414" s="8"/>
       <c r="AS414" s="8" t="str">
@@ -34302,14 +34064,14 @@
       <c r="U415" s="8"/>
       <c r="Z415" s="10"/>
       <c r="AB415" s="8" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="AC415" s="8" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AF415" s="39"/>
+      <c r="AF415" s="38"/>
       <c r="AP415" s="8"/>
       <c r="AQ415" s="8"/>
       <c r="AS415" s="8" t="str">
@@ -34331,14 +34093,14 @@
       <c r="U416" s="8"/>
       <c r="Z416" s="10"/>
       <c r="AB416" s="8" t="str">
-        <f t="shared" ref="AB416:AB479" si="35">IF(ISBLANK(AA416),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C416), "/", E416, "/config"))</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="AC416" s="8" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AF416" s="38"/>
+      <c r="AF416" s="39"/>
       <c r="AP416" s="8"/>
       <c r="AQ416" s="8"/>
       <c r="AS416" s="8" t="str">
@@ -34367,7 +34129,7 @@
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AF417" s="38"/>
+      <c r="AF417" s="39"/>
       <c r="AP417" s="8"/>
       <c r="AQ417" s="8"/>
       <c r="AS417" s="8" t="str">
@@ -34396,7 +34158,7 @@
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AF418" s="38"/>
+      <c r="AF418" s="39"/>
       <c r="AP418" s="8"/>
       <c r="AQ418" s="8"/>
       <c r="AS418" s="8" t="str">
@@ -34454,7 +34216,7 @@
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AF420" s="38"/>
+      <c r="AF420" s="39"/>
       <c r="AP420" s="8"/>
       <c r="AQ420" s="8"/>
       <c r="AS420" s="8" t="str">
@@ -34828,14 +34590,14 @@
         <v/>
       </c>
       <c r="AC433" s="8" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="AC433:AC496" si="36">IF(ISBLANK(AA433),  "", _xlfn.CONCAT(LOWER(C433), "/", E433))</f>
         <v/>
       </c>
       <c r="AF433" s="39"/>
       <c r="AP433" s="8"/>
       <c r="AQ433" s="8"/>
       <c r="AS433" s="8" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="AS433:AS496" si="37">IF(AND(ISBLANK(AO433), ISBLANK(AP433)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO433), "", _xlfn.CONCAT("[""mac"", """, AO433, """]")), IF(ISBLANK(AP433), "", _xlfn.CONCAT(", [""ip"", """, AP433, """]")), "]"))</f>
         <v/>
       </c>
     </row>
@@ -34857,14 +34619,14 @@
         <v/>
       </c>
       <c r="AC434" s="8" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AF434" s="39"/>
       <c r="AP434" s="8"/>
       <c r="AQ434" s="8"/>
       <c r="AS434" s="8" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
     </row>
@@ -34886,14 +34648,14 @@
         <v/>
       </c>
       <c r="AC435" s="8" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AF435" s="39"/>
       <c r="AP435" s="8"/>
       <c r="AQ435" s="8"/>
       <c r="AS435" s="8" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
     </row>
@@ -34915,14 +34677,14 @@
         <v/>
       </c>
       <c r="AC436" s="8" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AF436" s="39"/>
       <c r="AP436" s="8"/>
       <c r="AQ436" s="8"/>
       <c r="AS436" s="8" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
     </row>
@@ -34944,14 +34706,14 @@
         <v/>
       </c>
       <c r="AC437" s="8" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AF437" s="39"/>
       <c r="AP437" s="8"/>
       <c r="AQ437" s="8"/>
       <c r="AS437" s="8" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
     </row>
@@ -34973,14 +34735,14 @@
         <v/>
       </c>
       <c r="AC438" s="8" t="str">
-        <f t="shared" ref="AC438:AC501" si="36">IF(ISBLANK(AA438),  "", _xlfn.CONCAT(LOWER(C438), "/", E438))</f>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AF438" s="39"/>
       <c r="AP438" s="8"/>
       <c r="AQ438" s="8"/>
       <c r="AS438" s="8" t="str">
-        <f t="shared" ref="AS438:AS501" si="37">IF(AND(ISBLANK(AO438), ISBLANK(AP438)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO438), "", _xlfn.CONCAT("[""mac"", """, AO438, """]")), IF(ISBLANK(AP438), "", _xlfn.CONCAT(", [""ip"", """, AP438, """]")), "]"))</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
     </row>
@@ -36042,7 +35804,7 @@
       <c r="U475" s="8"/>
       <c r="Z475" s="10"/>
       <c r="AB475" s="8" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="AB475:AB538" si="38">IF(ISBLANK(AA475),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C475), "/", E475, "/config"))</f>
         <v/>
       </c>
       <c r="AC475" s="8" t="str">
@@ -36071,7 +35833,7 @@
       <c r="U476" s="8"/>
       <c r="Z476" s="10"/>
       <c r="AB476" s="8" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AC476" s="8" t="str">
@@ -36100,7 +35862,7 @@
       <c r="U477" s="8"/>
       <c r="Z477" s="10"/>
       <c r="AB477" s="8" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AC477" s="8" t="str">
@@ -36129,7 +35891,7 @@
       <c r="U478" s="8"/>
       <c r="Z478" s="10"/>
       <c r="AB478" s="8" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AC478" s="8" t="str">
@@ -36158,7 +35920,7 @@
       <c r="U479" s="8"/>
       <c r="Z479" s="10"/>
       <c r="AB479" s="8" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AC479" s="8" t="str">
@@ -36187,7 +35949,7 @@
       <c r="U480" s="8"/>
       <c r="Z480" s="10"/>
       <c r="AB480" s="8" t="str">
-        <f t="shared" ref="AB480:AB543" si="38">IF(ISBLANK(AA480),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C480), "/", E480, "/config"))</f>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AC480" s="8" t="str">
@@ -36613,6 +36375,7 @@
         <f>IF(ISBLANK(E495), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
+      <c r="H495" s="12"/>
       <c r="O495" s="8"/>
       <c r="P495" s="10"/>
       <c r="Q495" s="10"/>
@@ -36642,6 +36405,7 @@
         <f>IF(ISBLANK(E496), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
+      <c r="H496" s="12"/>
       <c r="O496" s="8"/>
       <c r="P496" s="10"/>
       <c r="Q496" s="10"/>
@@ -36684,14 +36448,14 @@
         <v/>
       </c>
       <c r="AC497" s="8" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="AC497:AC560" si="39">IF(ISBLANK(AA497),  "", _xlfn.CONCAT(LOWER(C497), "/", E497))</f>
         <v/>
       </c>
       <c r="AF497" s="39"/>
       <c r="AP497" s="8"/>
       <c r="AQ497" s="8"/>
       <c r="AS497" s="8" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="AS497:AS560" si="40">IF(AND(ISBLANK(AO497), ISBLANK(AP497)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO497), "", _xlfn.CONCAT("[""mac"", """, AO497, """]")), IF(ISBLANK(AP497), "", _xlfn.CONCAT(", [""ip"", """, AP497, """]")), "]"))</f>
         <v/>
       </c>
     </row>
@@ -36713,14 +36477,14 @@
         <v/>
       </c>
       <c r="AC498" s="8" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="AF498" s="39"/>
       <c r="AP498" s="8"/>
       <c r="AQ498" s="8"/>
       <c r="AS498" s="8" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
@@ -36742,14 +36506,14 @@
         <v/>
       </c>
       <c r="AC499" s="8" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="AF499" s="39"/>
       <c r="AP499" s="8"/>
       <c r="AQ499" s="8"/>
       <c r="AS499" s="8" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
@@ -36758,7 +36522,6 @@
         <f>IF(ISBLANK(E500), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
-      <c r="H500" s="12"/>
       <c r="O500" s="8"/>
       <c r="P500" s="10"/>
       <c r="Q500" s="10"/>
@@ -36772,14 +36535,14 @@
         <v/>
       </c>
       <c r="AC500" s="8" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="AF500" s="39"/>
       <c r="AP500" s="8"/>
       <c r="AQ500" s="8"/>
       <c r="AS500" s="8" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
@@ -36788,7 +36551,6 @@
         <f>IF(ISBLANK(E501), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
-      <c r="H501" s="12"/>
       <c r="O501" s="8"/>
       <c r="P501" s="10"/>
       <c r="Q501" s="10"/>
@@ -36796,20 +36558,19 @@
       <c r="S501" s="10"/>
       <c r="T501" s="10"/>
       <c r="U501" s="8"/>
-      <c r="Z501" s="10"/>
       <c r="AB501" s="8" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AC501" s="8" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="AF501" s="39"/>
       <c r="AP501" s="8"/>
       <c r="AQ501" s="8"/>
       <c r="AS501" s="8" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
@@ -36825,20 +36586,19 @@
       <c r="S502" s="10"/>
       <c r="T502" s="10"/>
       <c r="U502" s="8"/>
-      <c r="Z502" s="10"/>
       <c r="AB502" s="8" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AC502" s="8" t="str">
-        <f t="shared" ref="AC502:AC565" si="39">IF(ISBLANK(AA502),  "", _xlfn.CONCAT(LOWER(C502), "/", E502))</f>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="AF502" s="39"/>
       <c r="AP502" s="8"/>
       <c r="AQ502" s="8"/>
       <c r="AS502" s="8" t="str">
-        <f t="shared" ref="AS502:AS565" si="40">IF(AND(ISBLANK(AO502), ISBLANK(AP502)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO502), "", _xlfn.CONCAT("[""mac"", """, AO502, """]")), IF(ISBLANK(AP502), "", _xlfn.CONCAT(", [""ip"", """, AP502, """]")), "]"))</f>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
@@ -36854,7 +36614,6 @@
       <c r="S503" s="10"/>
       <c r="T503" s="10"/>
       <c r="U503" s="8"/>
-      <c r="Z503" s="10"/>
       <c r="AB503" s="8" t="str">
         <f t="shared" si="38"/>
         <v/>
@@ -36883,7 +36642,6 @@
       <c r="S504" s="10"/>
       <c r="T504" s="10"/>
       <c r="U504" s="8"/>
-      <c r="Z504" s="10"/>
       <c r="AB504" s="8" t="str">
         <f t="shared" si="38"/>
         <v/>
@@ -36905,6 +36663,7 @@
         <f>IF(ISBLANK(E505), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
+      <c r="G505" s="12"/>
       <c r="O505" s="8"/>
       <c r="P505" s="10"/>
       <c r="Q505" s="10"/>
@@ -36912,7 +36671,6 @@
       <c r="S505" s="10"/>
       <c r="T505" s="10"/>
       <c r="U505" s="8"/>
-      <c r="Z505" s="10"/>
       <c r="AB505" s="8" t="str">
         <f t="shared" si="38"/>
         <v/>
@@ -37046,7 +36804,6 @@
         <f>IF(ISBLANK(E510), "", Table2[[#This Row],[unique_id]])</f>
         <v/>
       </c>
-      <c r="G510" s="12"/>
       <c r="O510" s="8"/>
       <c r="P510" s="10"/>
       <c r="Q510" s="10"/>
@@ -37867,7 +37624,7 @@
       <c r="T539" s="10"/>
       <c r="U539" s="8"/>
       <c r="AB539" s="8" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="AB539:AB602" si="41">IF(ISBLANK(AA539),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C539), "/", E539, "/config"))</f>
         <v/>
       </c>
       <c r="AC539" s="8" t="str">
@@ -37895,7 +37652,7 @@
       <c r="T540" s="10"/>
       <c r="U540" s="8"/>
       <c r="AB540" s="8" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="AC540" s="8" t="str">
@@ -37923,7 +37680,7 @@
       <c r="T541" s="10"/>
       <c r="U541" s="8"/>
       <c r="AB541" s="8" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="AC541" s="8" t="str">
@@ -37951,7 +37708,7 @@
       <c r="T542" s="10"/>
       <c r="U542" s="8"/>
       <c r="AB542" s="8" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="AC542" s="8" t="str">
@@ -37979,7 +37736,7 @@
       <c r="T543" s="10"/>
       <c r="U543" s="8"/>
       <c r="AB543" s="8" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="AC543" s="8" t="str">
@@ -38007,7 +37764,7 @@
       <c r="T544" s="10"/>
       <c r="U544" s="8"/>
       <c r="AB544" s="8" t="str">
-        <f t="shared" ref="AB544:AB607" si="41">IF(ISBLANK(AA544),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C544), "/", E544, "/config"))</f>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="AC544" s="8" t="str">
@@ -38487,14 +38244,14 @@
         <v/>
       </c>
       <c r="AC561" s="8" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="AC561:AC624" si="42">IF(ISBLANK(AA561),  "", _xlfn.CONCAT(LOWER(C561), "/", E561))</f>
         <v/>
       </c>
       <c r="AF561" s="39"/>
       <c r="AP561" s="8"/>
       <c r="AQ561" s="8"/>
       <c r="AS561" s="8" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="AS561:AS624" si="43">IF(AND(ISBLANK(AO561), ISBLANK(AP561)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO561), "", _xlfn.CONCAT("[""mac"", """, AO561, """]")), IF(ISBLANK(AP561), "", _xlfn.CONCAT(", [""ip"", """, AP561, """]")), "]"))</f>
         <v/>
       </c>
     </row>
@@ -38515,14 +38272,14 @@
         <v/>
       </c>
       <c r="AC562" s="8" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AF562" s="39"/>
       <c r="AP562" s="8"/>
       <c r="AQ562" s="8"/>
       <c r="AS562" s="8" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -38543,14 +38300,14 @@
         <v/>
       </c>
       <c r="AC563" s="8" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AF563" s="39"/>
       <c r="AP563" s="8"/>
       <c r="AQ563" s="8"/>
       <c r="AS563" s="8" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -38571,14 +38328,14 @@
         <v/>
       </c>
       <c r="AC564" s="8" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AF564" s="39"/>
       <c r="AP564" s="8"/>
       <c r="AQ564" s="8"/>
       <c r="AS564" s="8" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -38599,14 +38356,14 @@
         <v/>
       </c>
       <c r="AC565" s="8" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AF565" s="39"/>
       <c r="AP565" s="8"/>
       <c r="AQ565" s="8"/>
       <c r="AS565" s="8" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -38627,14 +38384,14 @@
         <v/>
       </c>
       <c r="AC566" s="8" t="str">
-        <f t="shared" ref="AC566:AC629" si="42">IF(ISBLANK(AA566),  "", _xlfn.CONCAT(LOWER(C566), "/", E566))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AF566" s="39"/>
       <c r="AP566" s="8"/>
       <c r="AQ566" s="8"/>
       <c r="AS566" s="8" t="str">
-        <f t="shared" ref="AS566:AS629" si="43">IF(AND(ISBLANK(AO566), ISBLANK(AP566)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO566), "", _xlfn.CONCAT("[""mac"", """, AO566, """]")), IF(ISBLANK(AP566), "", _xlfn.CONCAT(", [""ip"", """, AP566, """]")), "]"))</f>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -39659,7 +39416,7 @@
       <c r="T603" s="10"/>
       <c r="U603" s="8"/>
       <c r="AB603" s="8" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="AB603:AB666" si="44">IF(ISBLANK(AA603),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C603), "/", E603, "/config"))</f>
         <v/>
       </c>
       <c r="AC603" s="8" t="str">
@@ -39687,7 +39444,7 @@
       <c r="T604" s="10"/>
       <c r="U604" s="8"/>
       <c r="AB604" s="8" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="AC604" s="8" t="str">
@@ -39715,7 +39472,7 @@
       <c r="T605" s="10"/>
       <c r="U605" s="8"/>
       <c r="AB605" s="8" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="AC605" s="8" t="str">
@@ -39743,7 +39500,7 @@
       <c r="T606" s="10"/>
       <c r="U606" s="8"/>
       <c r="AB606" s="8" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="AC606" s="8" t="str">
@@ -39771,7 +39528,7 @@
       <c r="T607" s="10"/>
       <c r="U607" s="8"/>
       <c r="AB607" s="8" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="AC607" s="8" t="str">
@@ -39799,7 +39556,7 @@
       <c r="T608" s="10"/>
       <c r="U608" s="8"/>
       <c r="AB608" s="8" t="str">
-        <f t="shared" ref="AB608:AB671" si="44">IF(ISBLANK(AA608),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C608), "/", E608, "/config"))</f>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="AC608" s="8" t="str">
@@ -40279,14 +40036,14 @@
         <v/>
       </c>
       <c r="AC625" s="8" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" ref="AC625:AC688" si="45">IF(ISBLANK(AA625),  "", _xlfn.CONCAT(LOWER(C625), "/", E625))</f>
         <v/>
       </c>
       <c r="AF625" s="39"/>
       <c r="AP625" s="8"/>
       <c r="AQ625" s="8"/>
       <c r="AS625" s="8" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" ref="AS625:AS688" si="46">IF(AND(ISBLANK(AO625), ISBLANK(AP625)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO625), "", _xlfn.CONCAT("[""mac"", """, AO625, """]")), IF(ISBLANK(AP625), "", _xlfn.CONCAT(", [""ip"", """, AP625, """]")), "]"))</f>
         <v/>
       </c>
     </row>
@@ -40307,14 +40064,14 @@
         <v/>
       </c>
       <c r="AC626" s="8" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AF626" s="39"/>
       <c r="AP626" s="8"/>
       <c r="AQ626" s="8"/>
       <c r="AS626" s="8" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
     </row>
@@ -40335,14 +40092,14 @@
         <v/>
       </c>
       <c r="AC627" s="8" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AF627" s="39"/>
       <c r="AP627" s="8"/>
       <c r="AQ627" s="8"/>
       <c r="AS627" s="8" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
     </row>
@@ -40363,14 +40120,14 @@
         <v/>
       </c>
       <c r="AC628" s="8" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AF628" s="39"/>
       <c r="AP628" s="8"/>
       <c r="AQ628" s="8"/>
       <c r="AS628" s="8" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
     </row>
@@ -40391,14 +40148,14 @@
         <v/>
       </c>
       <c r="AC629" s="8" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AF629" s="39"/>
       <c r="AP629" s="8"/>
       <c r="AQ629" s="8"/>
       <c r="AS629" s="8" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
     </row>
@@ -40419,14 +40176,14 @@
         <v/>
       </c>
       <c r="AC630" s="8" t="str">
-        <f t="shared" ref="AC630:AC693" si="45">IF(ISBLANK(AA630),  "", _xlfn.CONCAT(LOWER(C630), "/", E630))</f>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AF630" s="39"/>
       <c r="AP630" s="8"/>
       <c r="AQ630" s="8"/>
       <c r="AS630" s="8" t="str">
-        <f t="shared" ref="AS630:AS693" si="46">IF(AND(ISBLANK(AO630), ISBLANK(AP630)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO630), "", _xlfn.CONCAT("[""mac"", """, AO630, """]")), IF(ISBLANK(AP630), "", _xlfn.CONCAT(", [""ip"", """, AP630, """]")), "]"))</f>
+        <f t="shared" si="46"/>
         <v/>
       </c>
     </row>
@@ -41451,7 +41208,7 @@
       <c r="T667" s="10"/>
       <c r="U667" s="8"/>
       <c r="AB667" s="8" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" ref="AB667:AB695" si="47">IF(ISBLANK(AA667),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C667), "/", E667, "/config"))</f>
         <v/>
       </c>
       <c r="AC667" s="8" t="str">
@@ -41479,7 +41236,7 @@
       <c r="T668" s="10"/>
       <c r="U668" s="8"/>
       <c r="AB668" s="8" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="AC668" s="8" t="str">
@@ -41507,7 +41264,7 @@
       <c r="T669" s="10"/>
       <c r="U669" s="8"/>
       <c r="AB669" s="8" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="AC669" s="8" t="str">
@@ -41535,7 +41292,7 @@
       <c r="T670" s="10"/>
       <c r="U670" s="8"/>
       <c r="AB670" s="8" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="AC670" s="8" t="str">
@@ -41563,7 +41320,7 @@
       <c r="T671" s="10"/>
       <c r="U671" s="8"/>
       <c r="AB671" s="8" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="AC671" s="8" t="str">
@@ -41591,7 +41348,7 @@
       <c r="T672" s="10"/>
       <c r="U672" s="8"/>
       <c r="AB672" s="8" t="str">
-        <f t="shared" ref="AB672:AB700" si="47">IF(ISBLANK(AA672),  "", _xlfn.CONCAT("haas/entity/sensor/", LOWER(C672), "/", E672, "/config"))</f>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="AC672" s="8" t="str">
@@ -42071,14 +41828,14 @@
         <v/>
       </c>
       <c r="AC689" s="8" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="AC689:AC695" si="48">IF(ISBLANK(AA689),  "", _xlfn.CONCAT(LOWER(C689), "/", E689))</f>
         <v/>
       </c>
       <c r="AF689" s="39"/>
       <c r="AP689" s="8"/>
       <c r="AQ689" s="8"/>
       <c r="AS689" s="8" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" ref="AS689:AS695" si="49">IF(AND(ISBLANK(AO689), ISBLANK(AP689)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO689), "", _xlfn.CONCAT("[""mac"", """, AO689, """]")), IF(ISBLANK(AP689), "", _xlfn.CONCAT(", [""ip"", """, AP689, """]")), "]"))</f>
         <v/>
       </c>
     </row>
@@ -42099,14 +41856,14 @@
         <v/>
       </c>
       <c r="AC690" s="8" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AF690" s="39"/>
       <c r="AP690" s="8"/>
       <c r="AQ690" s="8"/>
       <c r="AS690" s="8" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
     </row>
@@ -42127,14 +41884,14 @@
         <v/>
       </c>
       <c r="AC691" s="8" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AF691" s="39"/>
       <c r="AP691" s="8"/>
       <c r="AQ691" s="8"/>
       <c r="AS691" s="8" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
     </row>
@@ -42155,14 +41912,14 @@
         <v/>
       </c>
       <c r="AC692" s="8" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AF692" s="39"/>
       <c r="AP692" s="8"/>
       <c r="AQ692" s="8"/>
       <c r="AS692" s="8" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
     </row>
@@ -42183,14 +41940,14 @@
         <v/>
       </c>
       <c r="AC693" s="8" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AF693" s="39"/>
       <c r="AP693" s="8"/>
       <c r="AQ693" s="8"/>
       <c r="AS693" s="8" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
     </row>
@@ -42211,14 +41968,14 @@
         <v/>
       </c>
       <c r="AC694" s="8" t="str">
-        <f t="shared" ref="AC694:AC700" si="48">IF(ISBLANK(AA694),  "", _xlfn.CONCAT(LOWER(C694), "/", E694))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AF694" s="39"/>
       <c r="AP694" s="8"/>
       <c r="AQ694" s="8"/>
       <c r="AS694" s="8" t="str">
-        <f t="shared" ref="AS694:AS700" si="49">IF(AND(ISBLANK(AO694), ISBLANK(AP694)), "", _xlfn.CONCAT("[", IF(ISBLANK(AO694), "", _xlfn.CONCAT("[""mac"", """, AO694, """]")), IF(ISBLANK(AP694), "", _xlfn.CONCAT(", [""ip"", """, AP694, """]")), "]"))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
     </row>
@@ -42246,146 +42003,6 @@
       <c r="AP695" s="8"/>
       <c r="AQ695" s="8"/>
       <c r="AS695" s="8" t="str">
-        <f t="shared" si="49"/>
-        <v/>
-      </c>
-    </row>
-    <row r="696" spans="6:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F696" s="8" t="str">
-        <f>IF(ISBLANK(E696), "", Table2[[#This Row],[unique_id]])</f>
-        <v/>
-      </c>
-      <c r="O696" s="8"/>
-      <c r="P696" s="10"/>
-      <c r="Q696" s="10"/>
-      <c r="R696" s="10"/>
-      <c r="S696" s="10"/>
-      <c r="T696" s="10"/>
-      <c r="U696" s="8"/>
-      <c r="AB696" s="8" t="str">
-        <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="AC696" s="8" t="str">
-        <f t="shared" si="48"/>
-        <v/>
-      </c>
-      <c r="AF696" s="39"/>
-      <c r="AP696" s="8"/>
-      <c r="AQ696" s="8"/>
-      <c r="AS696" s="8" t="str">
-        <f t="shared" si="49"/>
-        <v/>
-      </c>
-    </row>
-    <row r="697" spans="6:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F697" s="8" t="str">
-        <f>IF(ISBLANK(E697), "", Table2[[#This Row],[unique_id]])</f>
-        <v/>
-      </c>
-      <c r="O697" s="8"/>
-      <c r="P697" s="10"/>
-      <c r="Q697" s="10"/>
-      <c r="R697" s="10"/>
-      <c r="S697" s="10"/>
-      <c r="T697" s="10"/>
-      <c r="U697" s="8"/>
-      <c r="AB697" s="8" t="str">
-        <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="AC697" s="8" t="str">
-        <f t="shared" si="48"/>
-        <v/>
-      </c>
-      <c r="AF697" s="39"/>
-      <c r="AP697" s="8"/>
-      <c r="AQ697" s="8"/>
-      <c r="AS697" s="8" t="str">
-        <f t="shared" si="49"/>
-        <v/>
-      </c>
-    </row>
-    <row r="698" spans="6:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F698" s="8" t="str">
-        <f>IF(ISBLANK(E698), "", Table2[[#This Row],[unique_id]])</f>
-        <v/>
-      </c>
-      <c r="O698" s="8"/>
-      <c r="P698" s="10"/>
-      <c r="Q698" s="10"/>
-      <c r="R698" s="10"/>
-      <c r="S698" s="10"/>
-      <c r="T698" s="10"/>
-      <c r="U698" s="8"/>
-      <c r="AB698" s="8" t="str">
-        <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="AC698" s="8" t="str">
-        <f t="shared" si="48"/>
-        <v/>
-      </c>
-      <c r="AF698" s="39"/>
-      <c r="AP698" s="8"/>
-      <c r="AQ698" s="8"/>
-      <c r="AS698" s="8" t="str">
-        <f t="shared" si="49"/>
-        <v/>
-      </c>
-    </row>
-    <row r="699" spans="6:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F699" s="8" t="str">
-        <f>IF(ISBLANK(E699), "", Table2[[#This Row],[unique_id]])</f>
-        <v/>
-      </c>
-      <c r="O699" s="8"/>
-      <c r="P699" s="10"/>
-      <c r="Q699" s="10"/>
-      <c r="R699" s="10"/>
-      <c r="S699" s="10"/>
-      <c r="T699" s="10"/>
-      <c r="U699" s="8"/>
-      <c r="AB699" s="8" t="str">
-        <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="AC699" s="8" t="str">
-        <f t="shared" si="48"/>
-        <v/>
-      </c>
-      <c r="AF699" s="39"/>
-      <c r="AP699" s="8"/>
-      <c r="AQ699" s="8"/>
-      <c r="AS699" s="8" t="str">
-        <f t="shared" si="49"/>
-        <v/>
-      </c>
-    </row>
-    <row r="700" spans="6:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F700" s="8" t="str">
-        <f>IF(ISBLANK(E700), "", Table2[[#This Row],[unique_id]])</f>
-        <v/>
-      </c>
-      <c r="O700" s="8"/>
-      <c r="P700" s="10"/>
-      <c r="Q700" s="10"/>
-      <c r="R700" s="10"/>
-      <c r="S700" s="10"/>
-      <c r="T700" s="10"/>
-      <c r="U700" s="8"/>
-      <c r="AB700" s="8" t="str">
-        <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="AC700" s="8" t="str">
-        <f t="shared" si="48"/>
-        <v/>
-      </c>
-      <c r="AF700" s="39"/>
-      <c r="AP700" s="8"/>
-      <c r="AQ700" s="8"/>
-      <c r="AS700" s="8" t="str">
         <f t="shared" si="49"/>
         <v/>
       </c>

</xml_diff>